<commit_message>
feat: add content url column to hobby table
취미 테이블에 컨텐츠 URL 컬럼 추가

#14
</commit_message>
<xml_diff>
--- a/asset/images/HollangWeeks52_table_desc.xlsx
+++ b/asset/images/HollangWeeks52_table_desc.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="88">
   <si>
     <t>취미</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>img_url</t>
+  </si>
+  <si>
+    <t>취미 컨텐츠 즐기기 URL</t>
+  </si>
+  <si>
+    <t>content_url</t>
   </si>
   <si>
     <t>취미 추천 횟수</t>
@@ -635,7 +641,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H104"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -812,7 +818,7 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -838,7 +844,7 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -855,16 +861,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
         <v>31</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -880,79 +886,79 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
@@ -969,16 +975,16 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -995,10 +1001,10 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -1021,16 +1027,16 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
@@ -1047,16 +1053,16 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
@@ -1073,16 +1079,16 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
         <v>30</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
         <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
-        <v>29</v>
       </c>
       <c r="F20" t="s">
         <v>14</v>
@@ -1098,67 +1104,67 @@
       <c r="A21" t="s">
         <v>12</v>
       </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
@@ -1184,7 +1190,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>47</v>
@@ -1196,7 +1202,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="F26" t="s">
         <v>14</v>
@@ -1213,16 +1219,16 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
         <v>50</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
         <v>51</v>
-      </c>
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" t="s">
-        <v>20</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -1239,16 +1245,16 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F28" t="s">
         <v>14</v>
@@ -1265,16 +1271,16 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
         <v>30</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
         <v>31</v>
-      </c>
-      <c r="D29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" t="s">
-        <v>29</v>
       </c>
       <c r="F29" t="s">
         <v>14</v>
@@ -1290,73 +1296,73 @@
       <c r="A30" t="s">
         <v>12</v>
       </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>3</v>
-      </c>
-      <c r="D32" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" t="s">
-        <v>6</v>
-      </c>
-      <c r="G32" t="s">
-        <v>7</v>
-      </c>
-      <c r="H32" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G33" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H33" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
@@ -1376,13 +1382,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -1402,19 +1408,19 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
         <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="F36" t="s">
         <v>14</v>
@@ -1431,16 +1437,16 @@
         <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
         <v>51</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
-        <v>20</v>
       </c>
       <c r="F37" t="s">
         <v>14</v>
@@ -1457,16 +1463,16 @@
         <v>12</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F38" t="s">
         <v>14</v>
@@ -1483,16 +1489,16 @@
         <v>12</v>
       </c>
       <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
         <v>30</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
         <v>31</v>
-      </c>
-      <c r="D39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" t="s">
-        <v>29</v>
       </c>
       <c r="F39" t="s">
         <v>14</v>
@@ -1508,73 +1514,73 @@
       <c r="A40" t="s">
         <v>12</v>
       </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" t="s">
-        <v>6</v>
-      </c>
-      <c r="G42" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G43" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H43" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
         <v>60</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>61</v>
-      </c>
-      <c r="C44" t="s">
-        <v>62</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -1594,19 +1600,19 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="F45" t="s">
         <v>14</v>
@@ -1623,16 +1629,16 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" t="s">
         <v>30</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
         <v>31</v>
-      </c>
-      <c r="D46" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" t="s">
-        <v>29</v>
       </c>
       <c r="F46" t="s">
         <v>14</v>
@@ -1648,73 +1654,73 @@
       <c r="A47" t="s">
         <v>12</v>
       </c>
+      <c r="B47" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" t="s">
+        <v>12</v>
+      </c>
+      <c r="H47" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49" t="s">
-        <v>2</v>
-      </c>
-      <c r="C49" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" t="s">
-        <v>5</v>
-      </c>
-      <c r="F49" t="s">
-        <v>6</v>
-      </c>
-      <c r="G49" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F50" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H50" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
@@ -1734,13 +1740,13 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -1760,7 +1766,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
         <v>45</v>
@@ -1786,19 +1792,19 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B54" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C54" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
       </c>
       <c r="E54" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="F54" t="s">
         <v>14</v>
@@ -1815,16 +1821,16 @@
         <v>12</v>
       </c>
       <c r="B55" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" t="s">
         <v>30</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" t="s">
         <v>31</v>
-      </c>
-      <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
-        <v>29</v>
       </c>
       <c r="F55" t="s">
         <v>14</v>
@@ -1840,79 +1846,79 @@
       <c r="A56" t="s">
         <v>12</v>
       </c>
+      <c r="B56" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" t="s">
+        <v>31</v>
+      </c>
+      <c r="F56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" t="s">
+        <v>12</v>
+      </c>
+      <c r="H56" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>1</v>
-      </c>
-      <c r="B58" t="s">
-        <v>2</v>
-      </c>
-      <c r="C58" t="s">
-        <v>3</v>
-      </c>
-      <c r="D58" t="s">
-        <v>4</v>
-      </c>
-      <c r="E58" t="s">
-        <v>5</v>
-      </c>
-      <c r="F58" t="s">
-        <v>6</v>
-      </c>
-      <c r="G58" t="s">
-        <v>7</v>
-      </c>
-      <c r="H58" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E59" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F59" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G59" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H59" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C60" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D60" t="s">
         <v>12</v>
       </c>
       <c r="E60" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="F60" t="s">
         <v>14</v>
@@ -1929,16 +1935,16 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="C61" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
       </c>
       <c r="E61" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="F61" t="s">
         <v>14</v>
@@ -1955,16 +1961,16 @@
         <v>12</v>
       </c>
       <c r="B62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" t="s">
         <v>30</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" t="s">
         <v>31</v>
-      </c>
-      <c r="D62" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" t="s">
-        <v>29</v>
       </c>
       <c r="F62" t="s">
         <v>14</v>
@@ -1980,73 +1986,73 @@
       <c r="A63" t="s">
         <v>12</v>
       </c>
+      <c r="B63" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" t="s">
+        <v>31</v>
+      </c>
+      <c r="F63" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" t="s">
-        <v>2</v>
-      </c>
-      <c r="C65" t="s">
-        <v>3</v>
-      </c>
-      <c r="D65" t="s">
-        <v>4</v>
-      </c>
-      <c r="E65" t="s">
-        <v>5</v>
-      </c>
-      <c r="F65" t="s">
-        <v>6</v>
-      </c>
-      <c r="G65" t="s">
-        <v>7</v>
-      </c>
-      <c r="H65" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E66" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F66" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G66" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H66" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
@@ -2066,13 +2072,13 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" t="s">
         <v>60</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>61</v>
-      </c>
-      <c r="C68" t="s">
-        <v>62</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
@@ -2092,13 +2098,13 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B69" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C69" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
@@ -2118,19 +2124,19 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C70" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="D70" t="s">
         <v>12</v>
       </c>
       <c r="E70" t="s">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="F70" t="s">
         <v>14</v>
@@ -2147,16 +2153,16 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="C71" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="D71" t="s">
         <v>12</v>
       </c>
       <c r="E71" t="s">
-        <v>29</v>
+        <v>74</v>
       </c>
       <c r="F71" t="s">
         <v>14</v>
@@ -2173,16 +2179,16 @@
         <v>12</v>
       </c>
       <c r="B72" t="s">
+        <v>29</v>
+      </c>
+      <c r="C72" t="s">
         <v>30</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" t="s">
         <v>31</v>
-      </c>
-      <c r="D72" t="s">
-        <v>12</v>
-      </c>
-      <c r="E72" t="s">
-        <v>29</v>
       </c>
       <c r="F72" t="s">
         <v>14</v>
@@ -2198,79 +2204,79 @@
       <c r="A73" t="s">
         <v>12</v>
       </c>
+      <c r="B73" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73" t="s">
+        <v>31</v>
+      </c>
+      <c r="F73" t="s">
+        <v>14</v>
+      </c>
+      <c r="G73" t="s">
+        <v>12</v>
+      </c>
+      <c r="H73" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>1</v>
-      </c>
-      <c r="B75" t="s">
-        <v>2</v>
-      </c>
-      <c r="C75" t="s">
-        <v>3</v>
-      </c>
-      <c r="D75" t="s">
-        <v>4</v>
-      </c>
-      <c r="E75" t="s">
-        <v>5</v>
-      </c>
-      <c r="F75" t="s">
-        <v>6</v>
-      </c>
-      <c r="G75" t="s">
-        <v>7</v>
-      </c>
-      <c r="H75" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>61</v>
+        <v>2</v>
       </c>
       <c r="C76" t="s">
-        <v>62</v>
+        <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E76" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F76" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G76" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H76" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C77" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
       </c>
       <c r="E77" t="s">
-        <v>75</v>
+        <v>13</v>
       </c>
       <c r="F77" t="s">
         <v>14</v>
@@ -2287,16 +2293,16 @@
         <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D78" t="s">
         <v>12</v>
       </c>
       <c r="E78" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="F78" t="s">
         <v>14</v>
@@ -2313,16 +2319,16 @@
         <v>12</v>
       </c>
       <c r="B79" t="s">
+        <v>29</v>
+      </c>
+      <c r="C79" t="s">
         <v>30</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" t="s">
         <v>31</v>
-      </c>
-      <c r="D79" t="s">
-        <v>12</v>
-      </c>
-      <c r="E79" t="s">
-        <v>29</v>
       </c>
       <c r="F79" t="s">
         <v>14</v>
@@ -2338,73 +2344,73 @@
       <c r="A80" t="s">
         <v>12</v>
       </c>
+      <c r="B80" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" t="s">
+        <v>33</v>
+      </c>
+      <c r="D80" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" t="s">
+        <v>31</v>
+      </c>
+      <c r="F80" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" t="s">
+        <v>12</v>
+      </c>
+      <c r="H80" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>1</v>
-      </c>
-      <c r="B82" t="s">
-        <v>2</v>
-      </c>
-      <c r="C82" t="s">
-        <v>3</v>
-      </c>
-      <c r="D82" t="s">
-        <v>4</v>
-      </c>
-      <c r="E82" t="s">
-        <v>5</v>
-      </c>
-      <c r="F82" t="s">
-        <v>6</v>
-      </c>
-      <c r="G82" t="s">
-        <v>7</v>
-      </c>
-      <c r="H82" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="C83" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E83" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F83" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G83" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H83" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C84" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
@@ -2424,13 +2430,13 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C85" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
@@ -2450,19 +2456,19 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="B86" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="C86" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="D86" t="s">
         <v>12</v>
       </c>
       <c r="E86" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="F86" t="s">
         <v>14</v>
@@ -2479,16 +2485,16 @@
         <v>12</v>
       </c>
       <c r="B87" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C87" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D87" t="s">
         <v>12</v>
       </c>
       <c r="E87" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
       <c r="F87" t="s">
         <v>14</v>
@@ -2505,16 +2511,16 @@
         <v>12</v>
       </c>
       <c r="B88" t="s">
+        <v>29</v>
+      </c>
+      <c r="C88" t="s">
         <v>30</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
+        <v>12</v>
+      </c>
+      <c r="E88" t="s">
         <v>31</v>
-      </c>
-      <c r="D88" t="s">
-        <v>12</v>
-      </c>
-      <c r="E88" t="s">
-        <v>29</v>
       </c>
       <c r="F88" t="s">
         <v>14</v>
@@ -2530,73 +2536,73 @@
       <c r="A89" t="s">
         <v>12</v>
       </c>
+      <c r="B89" t="s">
+        <v>32</v>
+      </c>
+      <c r="C89" t="s">
+        <v>33</v>
+      </c>
+      <c r="D89" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" t="s">
+        <v>31</v>
+      </c>
+      <c r="F89" t="s">
+        <v>14</v>
+      </c>
+      <c r="G89" t="s">
+        <v>12</v>
+      </c>
+      <c r="H89" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>1</v>
-      </c>
-      <c r="B91" t="s">
-        <v>2</v>
-      </c>
-      <c r="C91" t="s">
-        <v>3</v>
-      </c>
-      <c r="D91" t="s">
-        <v>4</v>
-      </c>
-      <c r="E91" t="s">
-        <v>5</v>
-      </c>
-      <c r="F91" t="s">
-        <v>6</v>
-      </c>
-      <c r="G91" t="s">
-        <v>7</v>
-      </c>
-      <c r="H91" t="s">
-        <v>8</v>
+        <v>84</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E92" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F92" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G92" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H92" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B93" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="C93" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D93" t="s">
         <v>12</v>
@@ -2616,19 +2622,19 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B94" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C94" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D94" t="s">
         <v>12</v>
       </c>
       <c r="E94" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="F94" t="s">
         <v>14</v>
@@ -2645,16 +2651,16 @@
         <v>12</v>
       </c>
       <c r="B95" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="C95" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="D95" t="s">
         <v>12</v>
       </c>
       <c r="E95" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="F95" t="s">
         <v>14</v>
@@ -2671,16 +2677,16 @@
         <v>12</v>
       </c>
       <c r="B96" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" t="s">
         <v>30</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" t="s">
         <v>31</v>
-      </c>
-      <c r="D96" t="s">
-        <v>12</v>
-      </c>
-      <c r="E96" t="s">
-        <v>29</v>
       </c>
       <c r="F96" t="s">
         <v>14</v>
@@ -2696,79 +2702,79 @@
       <c r="A97" t="s">
         <v>12</v>
       </c>
+      <c r="B97" t="s">
+        <v>32</v>
+      </c>
+      <c r="C97" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" t="s">
+        <v>12</v>
+      </c>
+      <c r="E97" t="s">
+        <v>31</v>
+      </c>
+      <c r="F97" t="s">
+        <v>14</v>
+      </c>
+      <c r="G97" t="s">
+        <v>12</v>
+      </c>
+      <c r="H97" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>1</v>
-      </c>
-      <c r="B99" t="s">
-        <v>2</v>
-      </c>
-      <c r="C99" t="s">
-        <v>3</v>
-      </c>
-      <c r="D99" t="s">
-        <v>4</v>
-      </c>
-      <c r="E99" t="s">
-        <v>5</v>
-      </c>
-      <c r="F99" t="s">
-        <v>6</v>
-      </c>
-      <c r="G99" t="s">
-        <v>7</v>
-      </c>
-      <c r="H99" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="D100" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E100" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F100" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G100" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H100" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B101" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C101" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D101" t="s">
         <v>12</v>
       </c>
       <c r="E101" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="F101" t="s">
         <v>14</v>
@@ -2785,16 +2791,16 @@
         <v>12</v>
       </c>
       <c r="B102" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C102" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="D102" t="s">
         <v>12</v>
       </c>
       <c r="E102" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F102" t="s">
         <v>14</v>
@@ -2808,6 +2814,32 @@
     </row>
     <row r="103">
       <c r="A103" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" t="s">
+        <v>85</v>
+      </c>
+      <c r="C103" t="s">
+        <v>86</v>
+      </c>
+      <c r="D103" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103" t="s">
+        <v>51</v>
+      </c>
+      <c r="F103" t="s">
+        <v>14</v>
+      </c>
+      <c r="G103" t="s">
+        <v>12</v>
+      </c>
+      <c r="H103" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>